<commit_message>
Actualizo Product Backlog y Seguimiento de Metricas
</commit_message>
<xml_diff>
--- a/Documentacion/Seguimiento/Metricas/Seguimiento de Metricas.xlsx
+++ b/Documentacion/Seguimiento/Metricas/Seguimiento de Metricas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="778" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="778" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Índice de Métricas Activas" sheetId="5" r:id="rId1"/>
@@ -936,6 +936,10 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -989,10 +993,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1063,6 +1063,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1202,6 +1203,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1316,7 +1318,7 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>59</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1386,6 +1388,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1500,7 +1503,7 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>30</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1516,12 +1519,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-678830784"/>
-        <c:axId val="-678675344"/>
+        <c:axId val="26994096"/>
+        <c:axId val="26996272"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-678830784"/>
+        <c:axId val="26994096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1558,7 +1561,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-678675344"/>
+        <c:crossAx val="26996272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1566,7 +1569,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-678675344"/>
+        <c:axId val="26996272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1617,7 +1620,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-678830784"/>
+        <c:crossAx val="26994096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1635,6 +1638,7 @@
         <c:idx val="1"/>
         <c:delete val="1"/>
       </c:legendEntry>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2484,7 +2488,7 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>59</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3392,12 +3396,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-478116224"/>
-        <c:axId val="-478123296"/>
+        <c:axId val="27001168"/>
+        <c:axId val="27008864"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-478116224"/>
+        <c:axId val="27001168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3434,7 +3438,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-478123296"/>
+        <c:crossAx val="27008864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3442,7 +3446,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-478123296"/>
+        <c:axId val="27008864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3493,7 +3497,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-478116224"/>
+        <c:crossAx val="27001168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3842,12 +3846,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="-478120032"/>
-        <c:axId val="-478112960"/>
+        <c:axId val="309764752"/>
+        <c:axId val="309766928"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="-478120032"/>
+        <c:axId val="309764752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3879,7 +3883,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3940,7 +3943,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-478112960"/>
+        <c:crossAx val="309766928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3948,7 +3951,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-478112960"/>
+        <c:axId val="309766928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4062,7 +4065,7 @@
             <a:endParaRPr lang="es-AR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-478120032"/>
+        <c:crossAx val="309764752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4471,9 +4474,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4492,9 +4493,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4513,9 +4512,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4534,9 +4531,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4555,9 +4550,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4576,9 +4569,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4597,9 +4588,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4618,9 +4607,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4639,9 +4626,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4660,9 +4645,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
@@ -4681,9 +4664,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4738,9 +4719,7 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-              </c:ext>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9524,7 +9503,7 @@
       <c r="B8" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="80" t="s">
+      <c r="C8" s="62" t="s">
         <v>79</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -9550,8 +9529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9598,11 +9577,11 @@
       <c r="C4" s="26"/>
     </row>
     <row r="5" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="61" t="s">
+      <c r="A5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
@@ -9769,10 +9748,10 @@
         <v>21</v>
       </c>
       <c r="B20" s="3">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="C20" s="31">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -9927,10 +9906,10 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="65"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="36"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -10081,7 +10060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -10122,36 +10101,36 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="79" t="s">
+      <c r="A5" s="61" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="79" t="s">
+      <c r="A22" s="61" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="79" t="s">
+      <c r="A23" s="61" t="s">
         <v>54</v>
       </c>
-      <c r="H23" s="79" t="s">
+      <c r="H23" s="61" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="79" t="s">
+      <c r="A40" s="61" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="79" t="s">
+      <c r="H40" s="61" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="79" t="s">
+      <c r="A59" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="H59" s="79" t="s">
+      <c r="H59" s="61" t="s">
         <v>59</v>
       </c>
     </row>
@@ -10210,30 +10189,30 @@
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="77" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="77"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="78"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="78"/>
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="H7" s="79"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
       <c r="B8" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="72" t="s">
+      <c r="C8" s="74" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="73"/>
-      <c r="H8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="76"/>
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
     </row>
@@ -10262,14 +10241,14 @@
       <c r="B10" s="51">
         <v>10</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="68" t="s">
         <v>69</v>
       </c>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="70"/>
       <c r="I10" s="52"/>
       <c r="J10" s="52"/>
     </row>
@@ -10280,14 +10259,14 @@
       <c r="B11" s="51">
         <v>1</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="67"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="68"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="70"/>
       <c r="I11" s="52"/>
       <c r="J11" s="52"/>
     </row>
@@ -10298,14 +10277,14 @@
       <c r="B12" s="51">
         <v>2</v>
       </c>
-      <c r="C12" s="66" t="s">
+      <c r="C12" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="D12" s="67"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="68"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="70"/>
       <c r="I12" s="52"/>
       <c r="J12" s="52"/>
     </row>
@@ -10316,14 +10295,14 @@
       <c r="B13" s="51">
         <v>1</v>
       </c>
-      <c r="C13" s="66" t="s">
+      <c r="C13" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="67"/>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
-      <c r="H13" s="68"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="70"/>
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
     </row>
@@ -10334,14 +10313,14 @@
       <c r="B14" s="51">
         <v>4</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="70"/>
       <c r="I14" s="52"/>
       <c r="J14" s="52"/>
     </row>
@@ -10352,14 +10331,14 @@
       <c r="B15" s="51">
         <v>0</v>
       </c>
-      <c r="C15" s="66" t="s">
+      <c r="C15" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="67"/>
-      <c r="H15" s="68"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="70"/>
       <c r="I15" s="52"/>
       <c r="J15" s="52"/>
     </row>
@@ -10370,14 +10349,14 @@
       <c r="B16" s="51">
         <v>4</v>
       </c>
-      <c r="C16" s="66" t="s">
+      <c r="C16" s="68" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="G16" s="67"/>
-      <c r="H16" s="68"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="70"/>
       <c r="I16" s="52"/>
       <c r="J16" s="52"/>
     </row>
@@ -10388,14 +10367,14 @@
       <c r="B17" s="51">
         <v>5</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="68" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="67"/>
-      <c r="F17" s="67"/>
-      <c r="G17" s="67"/>
-      <c r="H17" s="68"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="70"/>
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
     </row>
@@ -10406,14 +10385,14 @@
       <c r="B18" s="51">
         <v>5</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="68" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="68"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="70"/>
       <c r="I18" s="52"/>
       <c r="J18" s="52"/>
     </row>
@@ -10424,14 +10403,14 @@
       <c r="B19" s="51">
         <v>4</v>
       </c>
-      <c r="C19" s="66" t="s">
+      <c r="C19" s="68" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="68"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="70"/>
       <c r="I19" s="52"/>
       <c r="J19" s="52"/>
     </row>
@@ -10442,14 +10421,14 @@
       <c r="B20" s="51">
         <v>0</v>
       </c>
-      <c r="C20" s="66" t="s">
+      <c r="C20" s="68" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="68"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="70"/>
       <c r="I20" s="52"/>
       <c r="J20" s="52"/>
     </row>
@@ -10460,14 +10439,14 @@
       <c r="B21" s="51">
         <v>15</v>
       </c>
-      <c r="C21" s="66" t="s">
+      <c r="C21" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="68"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="70"/>
       <c r="I21" s="52"/>
       <c r="J21" s="52"/>
     </row>
@@ -10478,14 +10457,14 @@
       <c r="B22" s="55">
         <v>3</v>
       </c>
-      <c r="C22" s="69" t="s">
+      <c r="C22" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="70"/>
-      <c r="E22" s="70"/>
-      <c r="F22" s="70"/>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="73"/>
       <c r="I22" s="52"/>
       <c r="J22" s="52"/>
     </row>
@@ -10558,76 +10537,76 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="s">
+      <c r="A6" s="80" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="47"/>
       <c r="F6" s="47"/>
       <c r="G6" s="47"/>
       <c r="H6" s="47"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="80" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="78"/>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
-      <c r="G24" s="78"/>
-      <c r="H24" s="78"/>
+      <c r="B24" s="80"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="78" t="s">
+      <c r="A42" s="80" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="78"/>
-      <c r="C42" s="78"/>
-      <c r="D42" s="78"/>
-      <c r="E42" s="78"/>
-      <c r="F42" s="78"/>
-      <c r="G42" s="78"/>
-      <c r="H42" s="78"/>
+      <c r="B42" s="80"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="80"/>
+      <c r="F42" s="80"/>
+      <c r="G42" s="80"/>
+      <c r="H42" s="80"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="78" t="s">
+      <c r="A60" s="80" t="s">
         <v>57</v>
       </c>
-      <c r="B60" s="78"/>
-      <c r="C60" s="78"/>
-      <c r="D60" s="78"/>
-      <c r="E60" s="78"/>
-      <c r="F60" s="78"/>
-      <c r="G60" s="78"/>
-      <c r="H60" s="78"/>
+      <c r="B60" s="80"/>
+      <c r="C60" s="80"/>
+      <c r="D60" s="80"/>
+      <c r="E60" s="80"/>
+      <c r="F60" s="80"/>
+      <c r="G60" s="80"/>
+      <c r="H60" s="80"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="78" t="s">
+      <c r="A78" s="80" t="s">
         <v>58</v>
       </c>
-      <c r="B78" s="78"/>
-      <c r="C78" s="78"/>
-      <c r="D78" s="78"/>
-      <c r="E78" s="78"/>
-      <c r="F78" s="78"/>
-      <c r="G78" s="78"/>
-      <c r="H78" s="78"/>
+      <c r="B78" s="80"/>
+      <c r="C78" s="80"/>
+      <c r="D78" s="80"/>
+      <c r="E78" s="80"/>
+      <c r="F78" s="80"/>
+      <c r="G78" s="80"/>
+      <c r="H78" s="80"/>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="78" t="s">
+      <c r="A96" s="80" t="s">
         <v>59</v>
       </c>
-      <c r="B96" s="78"/>
-      <c r="C96" s="78"/>
-      <c r="D96" s="78"/>
-      <c r="E96" s="78"/>
-      <c r="F96" s="78"/>
-      <c r="G96" s="78"/>
-      <c r="H96" s="78"/>
+      <c r="B96" s="80"/>
+      <c r="C96" s="80"/>
+      <c r="D96" s="80"/>
+      <c r="E96" s="80"/>
+      <c r="F96" s="80"/>
+      <c r="G96" s="80"/>
+      <c r="H96" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="11">

</xml_diff>